<commit_message>
Update on Excel file data upload
</commit_message>
<xml_diff>
--- a/src/test/java/artworkFiles/ArtworkRequests.xlsx
+++ b/src/test/java/artworkFiles/ArtworkRequests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pepsico\LabelRight-Selenium 11Apr\LabelRight\src\test\java\artworkFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07955062-2BCC-4324-9B06-8097983B0A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C47FD28-965F-4520-BE4C-9561EC56BA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0E6DD3CD-8B68-4729-9D7F-0343F204AF42}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Package Type</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Primary</t>
+  </si>
+  <si>
+    <t>US-Social Beverages</t>
   </si>
 </sst>
 </file>
@@ -420,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A56B773-5C22-4993-8301-FFDAEEC589DA}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="132.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="146.28515625" bestFit="1" customWidth="1"/>
@@ -462,6 +465,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>